<commit_message>
actualizacion archivos planeacion anual
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_organizacional_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_organizacional_aammdd.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\plan de acción sos\Organización\Calidad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="procesos" sheetId="5" r:id="rId2"/>
     <sheet name="Productos" sheetId="7" r:id="rId3"/>
+    <sheet name="Funcional" sheetId="8" r:id="rId4"/>
+    <sheet name="Física" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="126">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -175,6 +182,225 @@
   </si>
   <si>
     <t>¿Se definió un objetivo para cada métrica registrada?</t>
+  </si>
+  <si>
+    <t>Reporte de Monitoreo</t>
+  </si>
+  <si>
+    <t>¿Se revisó que los hitos se encontraran completos?(Nombre del hito, fecha planeada y fecha real)</t>
+  </si>
+  <si>
+    <t>¿Se revisaron los resultados de las auditorias?</t>
+  </si>
+  <si>
+    <t>De acuerdo a dichos resultados, ¿se realizó el análisis de los mismos?</t>
+  </si>
+  <si>
+    <t>¿Se agregarón comentarios para el seguimiento de los riesgos ?</t>
+  </si>
+  <si>
+    <t>¿Se analizaron los riesgos de los proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se reviso el cumplimiento de acuerdos con proveedores tras la adquisición de productos?</t>
+  </si>
+  <si>
+    <t>¿Se revisaron los costos planeados en el plan de trabajo contra los reales?</t>
+  </si>
+  <si>
+    <t>¿Se reviso el esfuerzo planeado en el plan de trabajo contra el real?</t>
+  </si>
+  <si>
+    <t>¿Se reviso el cumplimiento de la entrega de servicio acorde a lo establecido?</t>
+  </si>
+  <si>
+    <t>Catalogo de Servicios</t>
+  </si>
+  <si>
+    <t>¿Se encuentran registrados todos los productos que maneja la empresa?</t>
+  </si>
+  <si>
+    <t>¿Los productos registrados cuentan con un nombre del producto?</t>
+  </si>
+  <si>
+    <t>¿Se tiene especificado el tiempo de ejecución estimado para cada uno de los productos, esto contempla la forma remota y presencial?</t>
+  </si>
+  <si>
+    <t>¿Todos los productos cuentan con un costo de compra al proveedor?</t>
+  </si>
+  <si>
+    <t>¿Todos los productos cuentan con un precio de venta al publico?</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
+  </si>
+  <si>
+    <t>Plan de proyecto</t>
+  </si>
+  <si>
+    <t>¿Se Identificaró los Hitos y Entregables del proyecto?</t>
+  </si>
+  <si>
+    <t>¿Todos los Hitos/entregables cuentan con fecha de planeación y fecha real?</t>
+  </si>
+  <si>
+    <t>¿Esta definido el alcance del proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se definierón los recursos humanos necesarios para cubrir las necesidades del proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se encuentra definido la estructura organizacional del equipo de trabajo?</t>
+  </si>
+  <si>
+    <t>¿Se definieron las capacitaciones necesarias que el equipo de trabajo requiere para llevar a cabo el proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se definieron los participantes para las capacitaciones?</t>
+  </si>
+  <si>
+    <t>¿Se definió una fecha planeada para la ejecución de la capacitación?</t>
+  </si>
+  <si>
+    <t>¿Existe un plan de comunicación donde se definan los mensajes a transmitir durante el proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se definió una peridiocidad para el plan de comunicación?</t>
+  </si>
+  <si>
+    <t>¿Se definierón los participantes dentro del plan de comunicación?</t>
+  </si>
+  <si>
+    <t>¿Existe un calendario de actividades  donde se defina las actividades, responsables, fechas de ejecución y esfuerzo requerido para realizar dicha actividad?</t>
+  </si>
+  <si>
+    <t>¿Se definierón los recursos materiales necesarios para la ejecución del proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se asignó un responsable para cada riesgo identificado?</t>
+  </si>
+  <si>
+    <t>¿Existe un plan de mitigación para cada riesgo?</t>
+  </si>
+  <si>
+    <t>¿Cada riesgo cuenta con un plan de contingencia?</t>
+  </si>
+  <si>
+    <t>Verificación</t>
+  </si>
+  <si>
+    <t>Elementos de Configuración</t>
+  </si>
+  <si>
+    <t>¿Los elementos de configuración respetan el nombrado establecido en el documento Plan configuración?</t>
+  </si>
+  <si>
+    <t>¿Los elementos de configuración respetan la ubicación física definida en el documento Plan Configuración?</t>
+  </si>
+  <si>
+    <t>¿Se actualizarón apropiadamente los elementos de configuración afectados por algún cambio?</t>
+  </si>
+  <si>
+    <t>Línea Base</t>
+  </si>
+  <si>
+    <t>¿Se tiene identificada la versión de las linea base en los documentos?</t>
+  </si>
+  <si>
+    <t>¿Están identificados los elementos de configuración que forman parte de la Línea Base?</t>
+  </si>
+  <si>
+    <t>¿Los elementos de configuración que forman parte de la Línea Base se encuentran aprobados por el cliente?</t>
+  </si>
+  <si>
+    <t>¿Se actualizó la versión y el contenido de los documentos pertenecientes a la linea base ante algún cambio que afectara su estructura?</t>
+  </si>
+  <si>
+    <t>Control de Cambios</t>
+  </si>
+  <si>
+    <t>¿Se cuenta con la documentación necesaria para ejecutar el cambio solicitado?</t>
+  </si>
+  <si>
+    <t>Líneas Base</t>
+  </si>
+  <si>
+    <t>¿Se tienen almacenados todos los elementos pertenecientes a la linea base?</t>
+  </si>
+  <si>
+    <t>¿Se ha comunicado la creación/modificación de las líneas base?</t>
+  </si>
+  <si>
+    <t>¿El contenido de la linea base se ha generado de acuerdo a la ultima versión de las plantillas?</t>
+  </si>
+  <si>
+    <t>¿Se autorizo la solicitud de cambios por parte del CCC?</t>
+  </si>
+  <si>
+    <t>¿El cliente aprobó el cambio solicitado?</t>
+  </si>
+  <si>
+    <t>¿Se actualizaron todos los documentos que fueron involucrados en el documento control de cambios?</t>
+  </si>
+  <si>
+    <t>¿Se actualizó  la línea base de los productos afectadados?</t>
+  </si>
+  <si>
+    <t>Cambios</t>
+  </si>
+  <si>
+    <t>¿Se generó la solicitud de cambios?</t>
+  </si>
+  <si>
+    <t>¿Se revisarón y analizarón los cambios?</t>
+  </si>
+  <si>
+    <t>¿Se aprobarón o rechazarón los cambios a partir del analisís?</t>
+  </si>
+  <si>
+    <t>¿Se notificarón los cambios?</t>
+  </si>
+  <si>
+    <t>¿Actualizarón los documentos afectados por el cambio?</t>
+  </si>
+  <si>
+    <t>Planeación anual</t>
+  </si>
+  <si>
+    <t>¿Se generó el catalogo de productos?</t>
+  </si>
+  <si>
+    <t>¿Se generó el plan de proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se generó el plan de métricas?</t>
+  </si>
+  <si>
+    <t>¿Se aprobarón los documentos de planeación?</t>
+  </si>
+  <si>
+    <t>¿Se presentarón los planeas anuales al equipo de trabajo?</t>
+  </si>
+  <si>
+    <t>¿Se estimarón los costos anuales?</t>
+  </si>
+  <si>
+    <t>¿Se estimo un esfuerzo anual deejecución?</t>
+  </si>
+  <si>
+    <t>¿Se estimarón los gastos anuales de la empresa?</t>
+  </si>
+  <si>
+    <t>Auditoría Funcional</t>
+  </si>
+  <si>
+    <t>Auditoría Física</t>
   </si>
 </sst>
 </file>
@@ -187,7 +413,7 @@
     <numFmt numFmtId="166" formatCode="[$-80A]0%"/>
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;[Red]&quot;-&quot;[$$-80A]#,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -276,8 +502,60 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="American Typewriter"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="American Typewriter"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +634,62 @@
         <bgColor rgb="FFCFE7F5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE7F5"/>
+        <bgColor rgb="FFDCE6F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFEBF1DE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -489,6 +821,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
@@ -504,7 +965,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="100">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -590,6 +1051,40 @@
     <xf numFmtId="165" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -613,11 +1108,121 @@
     <xf numFmtId="165" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="15" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -691,7 +1296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -726,7 +1331,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -935,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ23"/>
+  <dimension ref="A1:AMJ40"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -957,68 +1562,68 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -1045,98 +1650,260 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19.5" customHeight="1">
-      <c r="B15" s="8" t="str">
-        <f>procesos!A11</f>
-        <v>Métricas y Monitoreo</v>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B15" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTA(procesos!C13:C17)</f>
         <v>0</v>
       </c>
       <c r="D15" s="10" t="e">
+        <f>COUNTIF(procesos!C23:C27,"x")/(COUNTIF((procesos!C23:C27),"x")+COUNTIF((procesos!D23:D27),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B16" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="9">
+        <f>COUNTA(procesos!C33:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="10" t="e">
+        <f>COUNTIF(procesos!C33:C37,"x")/(COUNTIF((procesos!C33:C37),"x")+COUNTIF((procesos!D33:D37),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" customHeight="1">
+      <c r="B17" s="8" t="str">
+        <f>procesos!A11</f>
+        <v>Métricas y Monitoreo</v>
+      </c>
+      <c r="C17" s="9">
+        <f>COUNTA(procesos!C13:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="10" t="e">
         <f>COUNTIF(procesos!C13:C17,"x")/(COUNTIF((procesos!C13:C17),"x")+COUNTIF((procesos!D13:D17),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" ht="12.75"/>
-    <row r="17" spans="2:4" s="5" customFormat="1" ht="12.75"/>
-    <row r="18" spans="2:4" ht="15.75">
-      <c r="B18" s="37" t="s">
+    <row r="18" spans="2:4" s="5" customFormat="1" ht="12.75"/>
+    <row r="19" spans="2:4" s="5" customFormat="1" ht="12.75"/>
+    <row r="20" spans="2:4" ht="15.75">
+      <c r="B20" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="6" t="s">
+      <c r="C20" s="94"/>
+      <c r="D20" s="95"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="8" t="s">
+    <row r="22" spans="2:4">
+      <c r="B22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C22" s="9">
         <f>COUNTA(Productos!C3:C7)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="10" t="e">
+      <c r="D22" s="10" t="e">
         <f>COUNTIF(Productos!C3:C7,"x")/(COUNTIF((Productos!C3:C7),"x")+COUNTIF((Productos!D3:D7),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="8" t="str">
+    <row r="23" spans="2:4">
+      <c r="B23" s="8" t="str">
         <f>Productos!A10</f>
         <v>Plan de Métricas</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C23" s="9">
         <f>COUNTA(Productos!C12:C19)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="10" t="e">
+      <c r="D23" s="10" t="e">
         <f>COUNTIF(Productos!C12:C19,"x")/(COUNTIF((Productos!C12:C19),"x")+COUNTIF((Productos!D12:D19),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="8" t="str">
+    <row r="24" spans="2:4">
+      <c r="B24" s="8" t="str">
         <f>Productos!A22</f>
         <v>Plan de Configuración</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C24" s="9">
         <f>COUNTA(Productos!C24:C30)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="10" t="e">
+      <c r="D24" s="10" t="e">
         <f>COUNTIF(Productos!C24:C30,"x")/(COUNTIF((Productos!C24:C30),"x")+COUNTIF((Productos!D24:D30),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="8" t="e">
-        <f>Productos!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="9">
-        <f>COUNTA(Productos!#REF!)</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="10" t="e">
-        <f>COUNTIF(Productos!#REF!,"x")/(COUNTIF((Productos!#REF!),"x")+COUNTIF((Productos!#REF!),"x"))</f>
-        <v>#REF!</v>
+    <row r="25" spans="2:4">
+      <c r="B25" s="8" t="str">
+        <f>Productos!A58</f>
+        <v>Plan de proyecto</v>
+      </c>
+      <c r="C25" s="9">
+        <f>COUNTA(Productos!C60:C78)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="10" t="e">
+        <f>COUNTIF(Productos!C60:C78,"x")/(COUNTIF((Productos!C60:C78),"x")+COUNTIF((Productos!D60:D78),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="8" t="str">
+        <f>Productos!A35</f>
+        <v>Reporte de Monitoreo</v>
+      </c>
+      <c r="C26" s="9">
+        <f>COUNTA(Productos!C37:C45)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="e">
+        <f>COUNTIF(Productos!C37:C45,"x")/(COUNTIF((Productos!C37:C45),"x")+COUNTIF((Productos!D37:D45),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="8" t="str">
+        <f>Productos!A47</f>
+        <v>Catalogo de Servicios</v>
+      </c>
+      <c r="C27" s="9">
+        <f>COUNTA(Productos!C49:C53)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="10" t="e">
+        <f>COUNTIF(Productos!C49:C53,"x")/(COUNTIF((Productos!C49:C53),"x")+COUNTIF((Productos!D49:D53),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="15.75">
+      <c r="B30" s="93" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="94"/>
+      <c r="D30" s="95"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="8" t="str">
+        <f>Funcional!A3</f>
+        <v>Líneas Base</v>
+      </c>
+      <c r="C32" s="9">
+        <f>COUNTA(Funcional!C4:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="10" t="e">
+        <f>COUNTIF(Funcional!C4:C6,"x")/(COUNTIF((Funcional!C4:C6),"x")+COUNTIF((Funcional!D4:D6),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="8" t="str">
+        <f>Funcional!A7</f>
+        <v>Control de Cambios</v>
+      </c>
+      <c r="C33" s="9">
+        <f>COUNTA(Funcional!C8:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="10" t="e">
+        <f>COUNTIF(Funcional!C8:C11,"x")/(COUNTIF((Funcional!C8:C11),"x")+COUNTIF((Funcional!D8:D11),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75">
+      <c r="B36" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="94"/>
+      <c r="D36" s="95"/>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="8" t="str">
+        <f>Física!A3</f>
+        <v>Elementos de Configuración</v>
+      </c>
+      <c r="C38" s="9">
+        <f>COUNTA(Física!C4:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="10" t="e">
+        <f>COUNTIF(Física!C4:C6,"x")/(COUNTIF((Física!C4:C6),"x")+COUNTIF((Física!D4:D6),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="8" t="str">
+        <f>Física!A7</f>
+        <v>Línea Base</v>
+      </c>
+      <c r="C39" s="9">
+        <f>COUNTA(Física!C8:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="10" t="e">
+        <f>COUNTIF(Física!C8:C11,"x")/(COUNTIF((Física!C8:C11),"x")+COUNTIF((Física!D8:D11),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="8" t="str">
+        <f>Física!A12</f>
+        <v>Control de Cambios</v>
+      </c>
+      <c r="C40" s="9">
+        <f>COUNTA(Física!C13:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="10" t="e">
+        <f>COUNTIF(Física!C13:C13,"x")/(COUNTIF((Física!C13:C13),"x")+COUNTIF((Física!D13:D13),"x"))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B18:D18"/>
+  <mergeCells count="10">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
@@ -1155,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:E25"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1169,22 +1936,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="40" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
@@ -1194,7 +1961,7 @@
       <c r="E2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="41"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1">
       <c r="A3" s="16">
@@ -1282,22 +2049,22 @@
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1"/>
     <row r="11" spans="1:6" s="13" customFormat="1">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="57"/>
+      <c r="C11" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="40" t="s">
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="23" t="s">
         <v>9</v>
       </c>
@@ -1307,7 +2074,7 @@
       <c r="E12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1">
       <c r="A13" s="16">
@@ -1372,61 +2139,209 @@
     <row r="18" spans="1:6" s="13" customFormat="1"/>
     <row r="19" spans="1:6" s="13" customFormat="1"/>
     <row r="20" spans="1:6" s="13" customFormat="1"/>
-    <row r="21" spans="1:6" s="13" customFormat="1"/>
-    <row r="22" spans="1:6" s="13" customFormat="1"/>
-    <row r="23" spans="1:6" s="13" customFormat="1"/>
-    <row r="24" spans="1:6" s="13" customFormat="1"/>
-    <row r="25" spans="1:6" s="13" customFormat="1">
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-    </row>
-    <row r="26" spans="1:6" s="13" customFormat="1"/>
-    <row r="27" spans="1:6" s="13" customFormat="1">
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+    <row r="21" spans="1:6" s="37" customFormat="1">
+      <c r="A21" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="37" customFormat="1">
+      <c r="A22" s="57"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="55"/>
+    </row>
+    <row r="23" spans="1:6" s="37" customFormat="1">
+      <c r="A23" s="16">
+        <v>1</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" s="37" customFormat="1">
+      <c r="A24" s="16">
+        <v>2</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="1:6" s="37" customFormat="1">
+      <c r="A25" s="16">
+        <v>3</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6" s="37" customFormat="1">
+      <c r="A26" s="16">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6" s="37" customFormat="1">
+      <c r="A27" s="16">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" s="13" customFormat="1"/>
     <row r="29" spans="1:6" s="13" customFormat="1"/>
     <row r="30" spans="1:6" s="13" customFormat="1"/>
-    <row r="31" spans="1:6" s="13" customFormat="1"/>
-    <row r="32" spans="1:6" s="13" customFormat="1"/>
-    <row r="33" spans="2:5" s="13" customFormat="1"/>
-    <row r="34" spans="2:5" s="13" customFormat="1"/>
-    <row r="35" spans="2:5" s="13" customFormat="1"/>
-    <row r="36" spans="2:5" s="13" customFormat="1"/>
-    <row r="37" spans="2:5" s="13" customFormat="1">
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-    </row>
-    <row r="38" spans="2:5" s="13" customFormat="1"/>
-    <row r="39" spans="2:5" s="13" customFormat="1">
+    <row r="31" spans="1:6" s="37" customFormat="1">
+      <c r="A31" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="57"/>
+      <c r="C31" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="58"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="37" customFormat="1">
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="55"/>
+    </row>
+    <row r="33" spans="1:6" s="37" customFormat="1">
+      <c r="A33" s="16">
+        <v>1</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="17"/>
+    </row>
+    <row r="34" spans="1:6" s="37" customFormat="1">
+      <c r="A34" s="16">
+        <v>2</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6" s="37" customFormat="1">
+      <c r="A35" s="16">
+        <v>3</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6" s="37" customFormat="1">
+      <c r="A36" s="16">
+        <v>4</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="17"/>
+    </row>
+    <row r="37" spans="1:6" s="37" customFormat="1">
+      <c r="A37" s="16">
+        <v>5</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6" s="13" customFormat="1"/>
+    <row r="39" spans="1:6" s="13" customFormat="1">
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
     </row>
-    <row r="40" spans="2:5" s="13" customFormat="1"/>
-    <row r="41" spans="2:5" s="13" customFormat="1"/>
-    <row r="42" spans="2:5" s="13" customFormat="1"/>
-    <row r="43" spans="2:5" s="13" customFormat="1"/>
-    <row r="44" spans="2:5" s="13" customFormat="1"/>
-    <row r="45" spans="2:5" s="13" customFormat="1"/>
-    <row r="46" spans="2:5" s="13" customFormat="1"/>
-    <row r="47" spans="2:5" s="13" customFormat="1"/>
-    <row r="48" spans="2:5" s="13" customFormat="1"/>
+    <row r="40" spans="1:6" s="13" customFormat="1"/>
+    <row r="41" spans="1:6" s="13" customFormat="1"/>
+    <row r="42" spans="1:6" s="13" customFormat="1"/>
+    <row r="43" spans="1:6" s="13" customFormat="1"/>
+    <row r="44" spans="1:6" s="13" customFormat="1"/>
+    <row r="45" spans="1:6" s="13" customFormat="1"/>
+    <row r="46" spans="1:6" s="13" customFormat="1"/>
+    <row r="47" spans="1:6" s="13" customFormat="1"/>
+    <row r="48" spans="1:6" s="13" customFormat="1"/>
     <row r="49" spans="2:5" s="13" customFormat="1"/>
     <row r="50" spans="2:5" s="13" customFormat="1"/>
     <row r="51" spans="2:5" s="13" customFormat="1"/>
     <row r="52" spans="2:5" s="13" customFormat="1"/>
     <row r="53" spans="2:5" s="13" customFormat="1">
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
     </row>
     <row r="54" spans="2:5" s="13" customFormat="1"/>
     <row r="55" spans="2:5" s="13" customFormat="1">
@@ -1528,16 +2443,20 @@
     <row r="147" s="13" customFormat="1"/>
     <row r="148" s="13" customFormat="1"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B37:E37"/>
     <mergeCell ref="A11:B12"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1547,10 +2466,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1560,22 +2479,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="40" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
@@ -1585,7 +2504,7 @@
       <c r="E2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="47"/>
+      <c r="F2" s="69"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="24">
@@ -1656,22 +2575,22 @@
       <c r="F8" s="21"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="57"/>
+      <c r="C10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="40" t="s">
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="23" t="s">
         <v>9</v>
       </c>
@@ -1681,7 +2600,7 @@
       <c r="E11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="16">
@@ -1780,22 +2699,22 @@
       <c r="F19" s="17"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="44" t="s">
+      <c r="B22" s="57"/>
+      <c r="C22" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="40" t="s">
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="23" t="s">
         <v>9</v>
       </c>
@@ -1805,7 +2724,7 @@
       <c r="E23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="41"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="16">
@@ -1897,19 +2816,849 @@
     <row r="32" spans="1:6" s="31" customFormat="1">
       <c r="B32" s="32"/>
     </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="65"/>
+      <c r="C35" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="65"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="67"/>
+    </row>
+    <row r="37" spans="1:6" ht="26.25">
+      <c r="A37" s="41">
+        <v>1</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="41">
+        <v>2</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="41">
+        <v>3</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="41">
+        <v>4</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="43"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="44">
+        <v>5</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="45"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="41">
+        <v>6</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="47"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="41">
+        <v>7</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="41">
+        <v>8</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="41">
+        <v>9</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="47"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="60"/>
+      <c r="C47" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1">
+      <c r="A48" s="60"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="61"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="48">
+        <v>1</v>
+      </c>
+      <c r="B49" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="48">
+        <v>2</v>
+      </c>
+      <c r="B50" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+    </row>
+    <row r="51" spans="1:6" ht="26.25">
+      <c r="A51" s="48">
+        <v>3</v>
+      </c>
+      <c r="B51" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="48">
+        <v>4</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="48">
+        <v>5</v>
+      </c>
+      <c r="B53" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+    </row>
+    <row r="58" spans="1:6" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A58" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="65"/>
+      <c r="C58" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1">
+      <c r="A59" s="65"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="67"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="72">
+        <v>1</v>
+      </c>
+      <c r="B60" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="74"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="74"/>
+      <c r="F60" s="75"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="74">
+        <v>2</v>
+      </c>
+      <c r="B61" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="74"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="75"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="74">
+        <v>3</v>
+      </c>
+      <c r="B62" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="75"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="74">
+        <v>4</v>
+      </c>
+      <c r="B63" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="75"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="74">
+        <v>6</v>
+      </c>
+      <c r="B64" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="74"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
+      <c r="F64" s="75"/>
+    </row>
+    <row r="65" spans="1:6" ht="30">
+      <c r="A65" s="74">
+        <v>7</v>
+      </c>
+      <c r="B65" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="74"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
+      <c r="F65" s="75"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="74">
+        <v>8</v>
+      </c>
+      <c r="B66" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="75"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="74">
+        <v>9</v>
+      </c>
+      <c r="B67" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="74"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
+      <c r="F67" s="75"/>
+    </row>
+    <row r="68" spans="1:6" ht="30">
+      <c r="A68" s="74">
+        <v>10</v>
+      </c>
+      <c r="B68" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="75"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="74">
+        <v>11</v>
+      </c>
+      <c r="B69" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="74"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
+      <c r="F69" s="75"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="74">
+        <v>12</v>
+      </c>
+      <c r="B70" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="74"/>
+      <c r="D70" s="74"/>
+      <c r="E70" s="74"/>
+      <c r="F70" s="75"/>
+    </row>
+    <row r="71" spans="1:6" ht="30">
+      <c r="A71" s="74">
+        <v>11</v>
+      </c>
+      <c r="B71" s="77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="74"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="75"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="74">
+        <v>12</v>
+      </c>
+      <c r="B72" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="74"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="75"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="74">
+        <v>13</v>
+      </c>
+      <c r="B73" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" s="74"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="74"/>
+      <c r="F73" s="75"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="74">
+        <v>14</v>
+      </c>
+      <c r="B74" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="75"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="96">
+        <v>15</v>
+      </c>
+      <c r="B75" s="99" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" s="74"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="75"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="74">
+        <v>16</v>
+      </c>
+      <c r="B76" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="98"/>
+      <c r="D76" s="98"/>
+      <c r="E76" s="98"/>
+      <c r="F76" s="98"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="74">
+        <v>17</v>
+      </c>
+      <c r="B77" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="98"/>
+      <c r="D77" s="98"/>
+      <c r="E77" s="98"/>
+      <c r="F77" s="98"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="74">
+        <v>18</v>
+      </c>
+      <c r="B78" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="98"/>
+      <c r="D78" s="98"/>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:F59"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A47:B48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="C47:E47"/>
     <mergeCell ref="A22:B23"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:F36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1">
+      <c r="A1" s="89"/>
+      <c r="B1" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="31.5">
+      <c r="A2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="80"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="82"/>
+    </row>
+    <row r="4" spans="1:6" ht="25.5">
+      <c r="A4" s="84">
+        <v>1</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="92"/>
+    </row>
+    <row r="5" spans="1:6" ht="25.5">
+      <c r="A5" s="84">
+        <v>2</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="87"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5">
+      <c r="A6" s="84">
+        <v>3</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="92"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="A7" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="79"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="82"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5">
+      <c r="A8" s="84">
+        <v>1</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="92"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="84">
+        <v>2</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="87"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5">
+      <c r="A10" s="84">
+        <v>3</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="87"/>
+    </row>
+    <row r="11" spans="1:6" ht="25.5">
+      <c r="A11" s="84">
+        <v>4</v>
+      </c>
+      <c r="B11" s="91" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="87"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1">
+      <c r="A1" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="31.5">
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="80"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="82"/>
+    </row>
+    <row r="4" spans="1:6" ht="26.25">
+      <c r="A4" s="84">
+        <v>1</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87"/>
+    </row>
+    <row r="5" spans="1:6" ht="26.25">
+      <c r="A5" s="84">
+        <v>2</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="87"/>
+    </row>
+    <row r="6" spans="1:6" ht="26.25">
+      <c r="A6" s="84">
+        <v>3</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="87"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="A7" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="79"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="82"/>
+    </row>
+    <row r="8" spans="1:6" ht="26.25">
+      <c r="A8" s="84">
+        <v>1</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="87"/>
+    </row>
+    <row r="9" spans="1:6" ht="26.25">
+      <c r="A9" s="84">
+        <v>2</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="87"/>
+    </row>
+    <row r="10" spans="1:6" ht="26.25">
+      <c r="A10" s="84">
+        <v>3</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="87"/>
+    </row>
+    <row r="11" spans="1:6" ht="39">
+      <c r="A11" s="84">
+        <v>4</v>
+      </c>
+      <c r="B11" s="85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="87"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="A12" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="79"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="82"/>
+    </row>
+    <row r="13" spans="1:6" ht="25.5">
+      <c r="A13" s="84">
+        <v>1</v>
+      </c>
+      <c r="B13" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="87"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>